<commit_message>
Add final data and print files
</commit_message>
<xml_diff>
--- a/PHY 222/Rydberg Constant/Data - Rydberg Constant.xlsx
+++ b/PHY 222/Rydberg Constant/Data - Rydberg Constant.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IISER\Labs\PHY 222\Rydberg Constant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4780E1E-BAA8-454C-A38A-278CC923860F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C231EAB-2203-4653-82FD-C3C7394ABABB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="44">
   <si>
     <t>Colour</t>
   </si>
@@ -224,6 +224,61 @@
   </si>
   <si>
     <t>Error %</t>
+  </si>
+  <si>
+    <t>(1.0991±0.0012)×10⁷</t>
+  </si>
+  <si>
+    <t>(1.1024±0.0011)×10⁷</t>
+  </si>
+  <si>
+    <t>(1.0992±0.0007)×10⁷</t>
+  </si>
+  <si>
+    <t>(1.1015±0.0005)×10⁷</t>
+  </si>
+  <si>
+    <t>(1.0932±0.0004)×10⁷</t>
+  </si>
+  <si>
+    <t>(1.0987±0.0003)×10⁷</t>
+  </si>
+  <si>
+    <t>(1.1020±0.0003)×10⁷</t>
+  </si>
+  <si>
+    <t>(1.0995±0.0003)×10⁷</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <r>
+      <t>R (m</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-1</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -507,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -524,14 +579,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -540,51 +589,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -605,6 +651,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -902,48 +969,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29" t="s">
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="30"/>
-      <c r="L1" s="22" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="23"/>
+      <c r="L1" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22" t="s">
+      <c r="M1" s="24"/>
+      <c r="N1" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="21" t="s">
+      <c r="O1" s="24"/>
+      <c r="P1" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="Q1" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="21" t="s">
+      <c r="S1" s="25" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="26"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -980,10 +1047,10 @@
       <c r="O2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="22"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="24"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -1541,16 +1608,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="P1:P2"/>
+    <mergeCell ref="Q1:Q2"/>
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="N1:O1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="P1:P2"/>
-    <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="R1:R2"/>
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="N1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1571,34 +1638,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31" t="s">
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="31" t="s">
+      <c r="L1" s="28" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="28"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1623,8 +1690,8 @@
       <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1657,7 +1724,7 @@
       <c r="J3" s="3">
         <v>20</v>
       </c>
-      <c r="K3" s="13">
+      <c r="K3" s="11">
         <v>15.045833333333327</v>
       </c>
       <c r="L3" s="3">
@@ -1695,7 +1762,7 @@
       <c r="J4" s="3">
         <v>12</v>
       </c>
-      <c r="K4" s="13">
+      <c r="K4" s="11">
         <v>16.891666666666666</v>
       </c>
       <c r="L4" s="3">
@@ -1733,7 +1800,7 @@
       <c r="J5" s="3">
         <v>48</v>
       </c>
-      <c r="K5" s="13">
+      <c r="K5" s="11">
         <v>20.591666666666669</v>
       </c>
       <c r="L5" s="3">
@@ -1771,7 +1838,7 @@
       <c r="J6" s="3">
         <v>26</v>
       </c>
-      <c r="K6" s="13">
+      <c r="K6" s="11">
         <v>23.150000000000006</v>
       </c>
       <c r="L6" s="3">
@@ -1809,7 +1876,7 @@
       <c r="J7" s="3">
         <v>44</v>
       </c>
-      <c r="K7" s="13">
+      <c r="K7" s="11">
         <v>54.420833333333334</v>
       </c>
       <c r="L7" s="3">
@@ -1847,7 +1914,7 @@
       <c r="J8" s="3">
         <v>58</v>
       </c>
-      <c r="K8" s="13">
+      <c r="K8" s="11">
         <v>45.099999999999994</v>
       </c>
       <c r="L8" s="3">
@@ -1873,11 +1940,11 @@
       <c r="F9" s="3">
         <v>14</v>
       </c>
-      <c r="G9" s="32"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="13">
+      <c r="G9" s="29"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="11">
         <v>141.11666666666667</v>
       </c>
       <c r="L9" s="3">
@@ -1903,11 +1970,11 @@
       <c r="F10" s="3">
         <v>5</v>
       </c>
-      <c r="G10" s="35"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
-      <c r="K10" s="13">
+      <c r="G10" s="32"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="11">
         <v>136.51666666666668</v>
       </c>
       <c r="L10" s="3">
@@ -1933,397 +2000,389 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34ABEBC-13E5-4A90-95F2-D4C9AFC8C20D}">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:G8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="8.88671875" style="15"/>
-    <col min="4" max="4" width="8.77734375" style="15" customWidth="1"/>
-    <col min="5" max="7" width="8.88671875" style="15"/>
-    <col min="8" max="8" width="8.88671875" style="15" customWidth="1"/>
-    <col min="9" max="9" width="12" style="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.88671875" style="15"/>
-    <col min="11" max="11" width="11.44140625" style="15" customWidth="1"/>
-    <col min="12" max="12" width="11" style="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="15"/>
+    <col min="1" max="3" width="8.88671875" style="13"/>
+    <col min="4" max="4" width="8.77734375" style="13" customWidth="1"/>
+    <col min="5" max="7" width="8.88671875" style="13"/>
+    <col min="8" max="8" width="8.88671875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="12" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="13"/>
+    <col min="11" max="11" width="11.44140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="13" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" s="10" customFormat="1" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>13</v>
+      <c r="L1" s="17" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="37">
         <v>1</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="37">
         <v>5</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="37">
         <v>193</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="37">
         <v>42</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="37">
         <v>223</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="37">
         <v>50</v>
       </c>
-      <c r="H2" s="16">
+      <c r="H2" s="38">
         <f>((F2+(G2/60)) - (D2+(E2/60)))/2</f>
         <v>15.066666666666677</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="39">
         <f>($C$14*SIN(PI()*H2/180) / B2) * 1000000000</f>
         <v>433.23795896739597</v>
       </c>
-      <c r="J2" s="15">
+      <c r="J2" s="37">
         <f>1000000000/(I2)</f>
         <v>2308200.3303299113</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="40">
         <f>(1/4 - 1/C2^2)</f>
         <v>0.21</v>
       </c>
-      <c r="L2" s="20">
-        <f>J2/K2</f>
-        <v>10991430.144428149</v>
+      <c r="L2" s="41" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="37">
         <v>1</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="37">
         <v>4</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="37">
         <v>191</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="37">
         <v>45</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="37">
         <v>225</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="37">
         <v>30</v>
       </c>
-      <c r="H3" s="16">
+      <c r="H3" s="38">
         <f t="shared" ref="H3:H8" si="0">((F3+(G3/60)) - (D3+(E3/60)))/2</f>
         <v>16.875</v>
       </c>
-      <c r="I3" s="17">
+      <c r="I3" s="39">
         <f t="shared" ref="I3:I8" si="1">($C$14*SIN(PI()*H3/180) / B3) * 1000000000</f>
         <v>483.80779542410392</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="37">
         <f t="shared" ref="J3:J8" si="2">1000000000/(I3)</f>
         <v>2066936.5178860009</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="40">
         <f t="shared" ref="K3:K8" si="3">(1/4 - 1/C3^2)</f>
         <v>0.1875</v>
       </c>
-      <c r="L3" s="20">
-        <f t="shared" ref="L3:L8" si="4">J3/K3</f>
-        <v>11023661.428725338</v>
+      <c r="L3" s="41" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="37">
         <v>1</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="37">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="37">
         <v>185</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="37">
         <v>30</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="37">
         <v>231</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="37">
         <v>47</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="38">
         <f t="shared" si="0"/>
         <v>23.141666666666666</v>
       </c>
-      <c r="I4" s="17">
+      <c r="I4" s="39">
         <f t="shared" si="1"/>
         <v>655.00987645007774</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="37">
         <f t="shared" si="2"/>
         <v>1526694.5369124003</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="40">
         <f t="shared" si="3"/>
         <v>0.1388888888888889</v>
       </c>
-      <c r="L4" s="20">
-        <f t="shared" si="4"/>
-        <v>10992200.665769281</v>
+      <c r="L4" s="41" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="37">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="37">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="37">
         <v>177</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="37">
         <v>26</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="37">
         <v>239</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="37">
         <v>56</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="38">
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="I5" s="17">
+      <c r="I5" s="39">
         <f t="shared" si="1"/>
         <v>432.3110484671011</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="37">
         <f t="shared" si="2"/>
         <v>2313149.3019801923</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="40">
         <f t="shared" si="3"/>
         <v>0.21</v>
       </c>
-      <c r="L5" s="20">
-        <f t="shared" si="4"/>
-        <v>11014996.676096154</v>
+      <c r="L5" s="41" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="37">
         <v>2</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="37">
         <v>4</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="37">
         <v>173</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="37">
         <v>5</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="37">
         <v>244</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="37">
         <v>45</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="38">
         <f t="shared" si="0"/>
         <v>35.833333333333329</v>
       </c>
-      <c r="I6" s="17">
+      <c r="I6" s="39">
         <f t="shared" si="1"/>
         <v>487.85786147495025</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="37">
         <f t="shared" si="2"/>
         <v>2049777.3613336482</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="40">
         <f t="shared" si="3"/>
         <v>0.1875</v>
       </c>
-      <c r="L6" s="20">
-        <f t="shared" si="4"/>
-        <v>10932145.92711279</v>
+      <c r="L6" s="41" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="37">
         <v>2</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="37">
         <v>3</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="37">
         <v>156</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="37">
         <v>44</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="37">
         <v>260</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="37">
         <v>26</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="38">
         <f t="shared" si="0"/>
         <v>51.850000000000009</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="39">
         <f t="shared" si="1"/>
         <v>655.33021417154089</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="37">
         <f t="shared" si="2"/>
         <v>1525948.2599382142</v>
       </c>
-      <c r="K7" s="18">
+      <c r="K7" s="40">
         <f t="shared" si="3"/>
         <v>0.1388888888888889</v>
       </c>
-      <c r="L7" s="20">
-        <f t="shared" si="4"/>
-        <v>10986827.471555142</v>
+      <c r="L7" s="41" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="37">
         <v>3</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="37">
         <v>5</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="37">
         <v>157</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="37">
         <v>19</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="37">
         <v>259</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="37">
         <v>26</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="38">
         <f t="shared" si="0"/>
         <v>51.058333333333337</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="39">
         <f t="shared" si="1"/>
         <v>432.10348619838277</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="37">
         <f t="shared" si="2"/>
         <v>2314260.4305230961</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="40">
         <f t="shared" si="3"/>
         <v>0.21</v>
       </c>
-      <c r="L8" s="20">
-        <f t="shared" si="4"/>
-        <v>11020287.764395697</v>
+      <c r="L8" s="41" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="L10" s="20">
-        <f>AVERAGE(L2:L8)</f>
-        <v>10994507.154011792</v>
-      </c>
-      <c r="M10" s="19">
-        <v>10970000</v>
-      </c>
+      <c r="K10" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L10" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" s="15"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="K11" s="15" t="s">
+      <c r="K11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="L11" s="17">
-        <f>(ABS(M10-L10)/M10)*100</f>
-        <v>0.22340158625151846</v>
+      <c r="L11" s="14">
+        <v>0.19</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="13">
         <v>15240</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="13" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="C14" s="15">
+      <c r="C14" s="13">
         <f>0.0254/C13</f>
         <v>1.6666666666666667E-6</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="13" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2337,193 +2396,193 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CDCDFB-C0F4-4A98-A886-222514D8422B}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="13">
         <v>1</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="13">
         <v>5</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="13">
         <v>193</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="13">
         <v>42</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="13">
         <v>223</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="13">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="13">
         <v>1</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="13">
         <v>4</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D3" s="13">
         <v>191</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="13">
         <v>45</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F3" s="13">
         <v>225</v>
       </c>
-      <c r="G3" s="15">
+      <c r="G3" s="13">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="13">
         <v>1</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="13">
         <v>3</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="13">
         <v>185</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="13">
         <v>30</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="13">
         <v>231</v>
       </c>
-      <c r="G4" s="15">
+      <c r="G4" s="13">
         <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="13">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="13">
         <v>5</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="13">
         <v>177</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="13">
         <v>26</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="13">
         <v>239</v>
       </c>
-      <c r="G5" s="15">
+      <c r="G5" s="13">
         <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="13">
         <v>2</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="13">
         <v>4</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="13">
         <v>173</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="13">
         <v>5</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="13">
         <v>244</v>
       </c>
-      <c r="G6" s="15">
+      <c r="G6" s="13">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="13">
         <v>3</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="13">
         <v>156</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="13">
         <v>44</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="13">
         <v>260</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="13">
         <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="13">
         <v>3</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="13">
         <v>5</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="13">
         <v>157</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="13">
         <v>19</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="13">
         <v>259</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="13">
         <v>26</v>
       </c>
     </row>

</xml_diff>